<commit_message>
Alterando nome da última coluna (adicionando ASV) e gerando novos arquivos de teste.
</commit_message>
<xml_diff>
--- a/example_files/eng/xlsx/1_threshold_application/output/thresholds.xlsx
+++ b/example_files/eng/xlsx/1_threshold_application/output/thresholds.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.058</v>
+        <v>6.47</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10.5028</v>
+        <v>7.502000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.454300000000001</v>
+        <v>5.3245</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.052</v>
+        <v>7.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>